<commit_message>
backup version for refactoring to flat schedule lists
</commit_message>
<xml_diff>
--- a/src/main/resources/t1.xlsx
+++ b/src/main/resources/t1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finn/repo/time-scheduler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDEADEC-5090-4641-9B3D-86585E329C8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3087C01E-E229-434E-A3CF-55084C729D96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19120" yWindow="5700" windowWidth="31740" windowHeight="16940" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
+    <workbookView xWindow="1140" yWindow="460" windowWidth="50060" windowHeight="28340" activeTab="1" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>person1</t>
-  </si>
-  <si>
     <t>System and Networks Lecture</t>
   </si>
   <si>
@@ -88,45 +85,6 @@
     <t>Preference3</t>
   </si>
   <si>
-    <t>Preference4</t>
-  </si>
-  <si>
-    <t>Preference5</t>
-  </si>
-  <si>
-    <t>Mon5pm</t>
-  </si>
-  <si>
-    <t>Mon5:00pm</t>
-  </si>
-  <si>
-    <t>Thurs 10 AM</t>
-  </si>
-  <si>
-    <t>Thurs 10:30 AM</t>
-  </si>
-  <si>
-    <t>Thurs 10:30 PM</t>
-  </si>
-  <si>
-    <t>Thurs 10:45 PM</t>
-  </si>
-  <si>
-    <t>fri-11.00</t>
-  </si>
-  <si>
-    <t>Preference6</t>
-  </si>
-  <si>
-    <t>Preference7</t>
-  </si>
-  <si>
-    <t>Preference8</t>
-  </si>
-  <si>
-    <t>Sun 0</t>
-  </si>
-  <si>
     <t>UTC+0</t>
   </si>
   <si>
@@ -152,6 +110,18 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>Mon 11 am</t>
+  </si>
+  <si>
+    <t>Mon1:00pm</t>
+  </si>
+  <si>
+    <t>Wednesday 1.30 PM</t>
   </si>
 </sst>
 </file>
@@ -176,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -196,9 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD6C2D6-AF9C-0D4D-9A30-20C849818904}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,25 +504,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -552,25 +530,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -578,25 +556,25 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -604,25 +582,25 @@
         <v>2.0833333333333301E-2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -630,25 +608,25 @@
         <v>3.125E-2</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -656,25 +634,25 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -682,25 +660,25 @@
         <v>5.2083333333333301E-2</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -708,25 +686,25 @@
         <v>6.25E-2</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -734,25 +712,25 @@
         <v>7.2916666666666699E-2</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -760,25 +738,25 @@
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -786,25 +764,25 @@
         <v>9.375E-2</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -812,25 +790,25 @@
         <v>0.104166666666667</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -838,25 +816,25 @@
         <v>0.114583333333333</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -864,25 +842,25 @@
         <v>0.125</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -890,25 +868,25 @@
         <v>0.13541666666666699</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -916,25 +894,25 @@
         <v>0.14583333333333301</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -942,25 +920,25 @@
         <v>0.15625</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -968,25 +946,25 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -994,25 +972,25 @@
         <v>0.17708333333333301</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1020,25 +998,25 @@
         <v>0.1875</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1046,25 +1024,25 @@
         <v>0.19791666666666699</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1072,25 +1050,25 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1098,25 +1076,25 @@
         <v>0.21875</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H23" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1124,25 +1102,25 @@
         <v>0.22916666666666699</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H24" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1150,25 +1128,25 @@
         <v>0.23958333333333301</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1176,25 +1154,25 @@
         <v>0.25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H26" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1202,25 +1180,25 @@
         <v>0.26041666666666702</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H27" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1228,25 +1206,25 @@
         <v>0.27083333333333298</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1254,25 +1232,25 @@
         <v>0.28125</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1280,25 +1258,25 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1306,25 +1284,25 @@
         <v>0.30208333333333298</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1332,25 +1310,25 @@
         <v>0.3125</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H32" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1358,25 +1336,25 @@
         <v>0.32291666666666702</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1384,10 +1362,10 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H34" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1395,10 +1373,10 @@
         <v>0.34375</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H35" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1406,10 +1384,10 @@
         <v>0.35416666666666702</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1417,10 +1395,10 @@
         <v>0.36458333333333298</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H37" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1428,22 +1406,22 @@
         <v>0.375</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H38" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1451,22 +1429,22 @@
         <v>0.38541666666666702</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H39" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1474,22 +1452,22 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-      <c r="F40" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1497,22 +1475,22 @@
         <v>0.40625</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H41" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1520,19 +1498,19 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>10</v>
+      <c r="F42" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H42" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1540,19 +1518,19 @@
         <v>0.42708333333333298</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D43" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" t="s">
-        <v>10</v>
+      <c r="F43" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H43" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1560,19 +1538,19 @@
         <v>0.4375</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D44" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" t="s">
-        <v>10</v>
+      <c r="F44" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H44" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1580,19 +1558,19 @@
         <v>0.44791666666666702</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>10</v>
+      <c r="F45" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H45" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1600,16 +1578,16 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H46" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1617,16 +1595,16 @@
         <v>0.46875</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H47" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1634,16 +1612,16 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H48" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1651,16 +1629,16 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H49" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1668,19 +1646,19 @@
         <v>0.5</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1688,19 +1666,19 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H51" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1708,19 +1686,19 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H52" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1728,19 +1706,19 @@
         <v>0.53125</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H53" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -1748,13 +1726,13 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="F54" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H54" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -1762,13 +1740,13 @@
         <v>0.55208333333333304</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
-      </c>
-      <c r="F55" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1776,13 +1754,13 @@
         <v>0.5625</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
-      </c>
-      <c r="F56" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H56" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -1790,13 +1768,13 @@
         <v>0.57291666666666696</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H57" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -1804,13 +1782,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -1818,13 +1796,13 @@
         <v>0.59375</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -1832,13 +1810,13 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1846,13 +1824,13 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -1860,16 +1838,16 @@
         <v>0.625</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H62" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -1877,16 +1855,16 @@
         <v>0.63541666666666696</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" t="s">
-        <v>4</v>
-      </c>
-      <c r="F63" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H63" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -1894,16 +1872,16 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" t="s">
-        <v>4</v>
-      </c>
-      <c r="F64" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -1911,16 +1889,16 @@
         <v>0.65625</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H65" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -1928,16 +1906,16 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H66" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -1945,16 +1923,16 @@
         <v>0.67708333333333304</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H67" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -1962,16 +1940,16 @@
         <v>0.6875</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
-      </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="F68" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H68" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -1979,16 +1957,16 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-      <c r="F69" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H69" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -1996,10 +1974,10 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H70" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2007,10 +1985,10 @@
         <v>0.71875</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H71" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2018,10 +1996,10 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H72" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2029,10 +2007,10 @@
         <v>0.73958333333333304</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H73" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2040,25 +2018,25 @@
         <v>0.75</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H74" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -2066,25 +2044,25 @@
         <v>0.76041666666666696</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H75" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -2092,25 +2070,25 @@
         <v>0.77083333333333304</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H76" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2118,25 +2096,25 @@
         <v>0.78125</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H77" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2144,25 +2122,25 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H78" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2170,25 +2148,25 @@
         <v>0.80208333333333304</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H79" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2196,25 +2174,25 @@
         <v>0.8125</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H80" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2222,25 +2200,25 @@
         <v>0.82291666666666696</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H81" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2248,25 +2226,25 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2274,25 +2252,25 @@
         <v>0.84375</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H83" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2300,25 +2278,25 @@
         <v>0.85416666666666696</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H84" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2326,25 +2304,25 @@
         <v>0.86458333333333304</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H85" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2352,25 +2330,25 @@
         <v>0.875</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H86" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2378,25 +2356,25 @@
         <v>0.88541666666666696</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H87" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2404,25 +2382,25 @@
         <v>0.89583333333333304</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H88" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2430,25 +2408,25 @@
         <v>0.90625</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H89" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2456,25 +2434,25 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H90" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2482,25 +2460,25 @@
         <v>0.92708333333333304</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H91" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2508,25 +2486,25 @@
         <v>0.9375</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H92" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2534,25 +2512,25 @@
         <v>0.94791666666666696</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H93" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2560,25 +2538,25 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H94" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -2586,25 +2564,25 @@
         <v>0.96875</v>
       </c>
       <c r="B95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H95" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -2612,25 +2590,25 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H96" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -2638,25 +2616,25 @@
         <v>0.98958333333333304</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H97" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2668,10 +2646,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD91671D-DED2-E74A-92AE-2A272D567A9A}">
-  <dimension ref="A1:B11"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2689,79 +2668,39 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enable recognition of dynamic aligned header in the input, the result now can be exported to excel files
</commit_message>
<xml_diff>
--- a/src/main/resources/t1.xlsx
+++ b/src/main/resources/t1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finn/repo/time-scheduler/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/finn/repo/meeting-scheduler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3087C01E-E229-434E-A3CF-55084C729D96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0406DB05-32EF-8C47-81DF-201ABD6E6389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="50060" windowHeight="28340" activeTab="1" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
+    <workbookView xWindow="1140" yWindow="460" windowWidth="16360" windowHeight="28340" xr2:uid="{B79D25B7-5550-B540-A36A-E2C0BE443EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +156,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,10 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +500,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,6 +1371,9 @@
       <c r="B34" t="s">
         <v>17</v>
       </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
       <c r="H34" t="s">
         <v>17</v>
       </c>
@@ -1375,6 +1385,9 @@
       <c r="B35" t="s">
         <v>17</v>
       </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
       <c r="H35" t="s">
         <v>17</v>
       </c>
@@ -1386,6 +1399,9 @@
       <c r="B36" t="s">
         <v>17</v>
       </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
       <c r="H36" t="s">
         <v>17</v>
       </c>
@@ -1397,6 +1413,9 @@
       <c r="B37" t="s">
         <v>17</v>
       </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
       <c r="H37" t="s">
         <v>17</v>
       </c>
@@ -1580,6 +1599,7 @@
       <c r="B46" t="s">
         <v>17</v>
       </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1597,6 +1617,7 @@
       <c r="B47" t="s">
         <v>17</v>
       </c>
+      <c r="C47" s="3"/>
       <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
@@ -1614,6 +1635,7 @@
       <c r="B48" t="s">
         <v>17</v>
       </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
@@ -1631,6 +1653,7 @@
       <c r="B49" t="s">
         <v>17</v>
       </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
@@ -1728,6 +1751,8 @@
       <c r="B54" t="s">
         <v>17</v>
       </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
       <c r="F54" s="2" t="s">
         <v>11</v>
       </c>
@@ -1742,6 +1767,8 @@
       <c r="B55" t="s">
         <v>17</v>
       </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
       <c r="F55" s="2" t="s">
         <v>11</v>
       </c>
@@ -1756,6 +1783,8 @@
       <c r="B56" t="s">
         <v>17</v>
       </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
       <c r="F56" s="2" t="s">
         <v>11</v>
       </c>
@@ -1770,6 +1799,8 @@
       <c r="B57" t="s">
         <v>17</v>
       </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
       <c r="F57" s="2" t="s">
         <v>11</v>
       </c>
@@ -1787,6 +1818,7 @@
       <c r="C58" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D58" s="3"/>
       <c r="H58" t="s">
         <v>17</v>
       </c>
@@ -1801,6 +1833,7 @@
       <c r="C59" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D59" s="3"/>
       <c r="H59" t="s">
         <v>17</v>
       </c>
@@ -1815,6 +1848,7 @@
       <c r="C60" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D60" s="3"/>
       <c r="H60" t="s">
         <v>17</v>
       </c>
@@ -1829,6 +1863,7 @@
       <c r="C61" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D61" s="3"/>
       <c r="H61" t="s">
         <v>17</v>
       </c>
@@ -1843,6 +1878,7 @@
       <c r="C62" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D62" s="3"/>
       <c r="F62" s="2" t="s">
         <v>11</v>
       </c>
@@ -1860,6 +1896,7 @@
       <c r="C63" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D63" s="3"/>
       <c r="F63" s="2" t="s">
         <v>11</v>
       </c>
@@ -1877,6 +1914,7 @@
       <c r="C64" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D64" s="3"/>
       <c r="F64" s="2" t="s">
         <v>11</v>
       </c>
@@ -1894,6 +1932,7 @@
       <c r="C65" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D65" s="3"/>
       <c r="F65" s="2" t="s">
         <v>11</v>
       </c>
@@ -2649,7 +2688,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>